<commit_message>
Updates to tech selection
</commit_message>
<xml_diff>
--- a/es_gui/apps/data_manager/_static/techs_database.xlsx
+++ b/es_gui/apps/data_manager/_static/techs_database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afurlan\Documents\QuESt\snl-quest-1.2.g\es_gui\apps\data_manager\_static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afurlan\Documents\QuESt\snl-quest\es_gui\apps\data_manager\_static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1113,10 +1113,10 @@
   <dimension ref="A1:CK51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BN10" sqref="BN10"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1405,7 +1405,7 @@
         <v>86</v>
       </c>
       <c r="N2" s="4">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="O2" s="4">
         <v>10</v>
@@ -1434,11 +1434,11 @@
       <c r="X2" s="3">
         <v>1</v>
       </c>
-      <c r="Y2" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>0.3</v>
+      <c r="Y2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.35">
@@ -1482,7 +1482,7 @@
         <v>86</v>
       </c>
       <c r="N3" s="4">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="O3" s="4">
         <v>10</v>
@@ -1511,11 +1511,11 @@
       <c r="X3" s="3">
         <v>1</v>
       </c>
-      <c r="Y3" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>0.3</v>
+      <c r="Y3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.35">
@@ -1559,7 +1559,7 @@
         <v>86</v>
       </c>
       <c r="N4" s="4">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="O4" s="4">
         <v>10</v>
@@ -1588,11 +1588,11 @@
       <c r="X4" s="3">
         <v>1</v>
       </c>
-      <c r="Y4" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>0.3</v>
+      <c r="Y4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:66" x14ac:dyDescent="0.35">
@@ -1636,7 +1636,7 @@
         <v>86</v>
       </c>
       <c r="N5" s="4">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="O5" s="4">
         <v>10</v>
@@ -1665,11 +1665,11 @@
       <c r="X5" s="3">
         <v>1</v>
       </c>
-      <c r="Y5" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z5" s="4">
-        <v>0.3</v>
+      <c r="Y5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.35">
@@ -1713,7 +1713,7 @@
         <v>86</v>
       </c>
       <c r="N6" s="4">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="O6" s="4">
         <v>10</v>
@@ -1742,11 +1742,11 @@
       <c r="X6" s="3">
         <v>1</v>
       </c>
-      <c r="Y6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z6" s="4">
-        <v>0.3</v>
+      <c r="Y6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:66" x14ac:dyDescent="0.35">
@@ -1790,7 +1790,7 @@
         <v>86</v>
       </c>
       <c r="N7" s="4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="O7" s="4">
         <v>10</v>
@@ -1819,11 +1819,11 @@
       <c r="X7" s="3">
         <v>1</v>
       </c>
-      <c r="Y7" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z7" s="4">
-        <v>0.3</v>
+      <c r="Y7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:66" x14ac:dyDescent="0.35">
@@ -1867,7 +1867,7 @@
         <v>86</v>
       </c>
       <c r="N8" s="4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="O8" s="4">
         <v>10</v>
@@ -1896,11 +1896,11 @@
       <c r="X8" s="3">
         <v>1</v>
       </c>
-      <c r="Y8" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z8" s="4">
-        <v>0.3</v>
+      <c r="Y8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:66" x14ac:dyDescent="0.35">
@@ -1944,7 +1944,7 @@
         <v>86</v>
       </c>
       <c r="N9" s="4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="O9" s="4">
         <v>10</v>
@@ -1973,11 +1973,11 @@
       <c r="X9" s="3">
         <v>1</v>
       </c>
-      <c r="Y9" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z9" s="4">
-        <v>0.3</v>
+      <c r="Y9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:66" x14ac:dyDescent="0.35">
@@ -2021,7 +2021,7 @@
         <v>86</v>
       </c>
       <c r="N10" s="4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="O10" s="4">
         <v>10</v>
@@ -2050,11 +2050,11 @@
       <c r="X10" s="3">
         <v>1</v>
       </c>
-      <c r="Y10" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z10" s="4">
-        <v>0.3</v>
+      <c r="Y10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.35">
@@ -2098,7 +2098,7 @@
         <v>86</v>
       </c>
       <c r="N11" s="4">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="O11" s="4">
         <v>10</v>
@@ -2127,11 +2127,11 @@
       <c r="X11" s="3">
         <v>1</v>
       </c>
-      <c r="Y11" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z11" s="4">
-        <v>0.3</v>
+      <c r="Y11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.35">
@@ -2175,7 +2175,7 @@
         <v>82</v>
       </c>
       <c r="N12" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O12" s="4">
         <v>10</v>
@@ -2199,16 +2199,16 @@
         <v>0.51249999999999996</v>
       </c>
       <c r="W12" s="3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="X12" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="Y12" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z12" s="4">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.35">
@@ -2252,7 +2252,7 @@
         <v>82</v>
       </c>
       <c r="N13" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O13" s="4">
         <v>10</v>
@@ -2276,16 +2276,16 @@
         <v>0.51249999999999996</v>
       </c>
       <c r="W13" s="3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="X13" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="Y13" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z13" s="4">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.35">
@@ -2329,7 +2329,7 @@
         <v>86</v>
       </c>
       <c r="N14" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O14" s="4">
         <v>10</v>
@@ -2358,11 +2358,11 @@
       <c r="X14" s="3">
         <v>1</v>
       </c>
-      <c r="Y14" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z14" s="4">
-        <v>0.3</v>
+      <c r="Y14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.35">
@@ -2406,7 +2406,7 @@
         <v>86</v>
       </c>
       <c r="N15" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O15" s="4">
         <v>10</v>
@@ -2435,11 +2435,11 @@
       <c r="X15" s="3">
         <v>1</v>
       </c>
-      <c r="Y15" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z15" s="4">
-        <v>0.3</v>
+      <c r="Y15" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.35">
@@ -2483,7 +2483,7 @@
         <v>86</v>
       </c>
       <c r="N16" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O16" s="4">
         <v>10</v>
@@ -2512,11 +2512,11 @@
       <c r="X16" s="3">
         <v>1</v>
       </c>
-      <c r="Y16" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z16" s="4">
-        <v>0.3</v>
+      <c r="Y16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.35">
@@ -2560,7 +2560,7 @@
         <v>86</v>
       </c>
       <c r="N17" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O17" s="4">
         <v>10</v>
@@ -2589,11 +2589,11 @@
       <c r="X17" s="3">
         <v>1</v>
       </c>
-      <c r="Y17" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z17" s="4">
-        <v>0.3</v>
+      <c r="Y17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.35">
@@ -2637,7 +2637,7 @@
         <v>86</v>
       </c>
       <c r="N18" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O18" s="4">
         <v>10</v>
@@ -2666,11 +2666,11 @@
       <c r="X18" s="3">
         <v>1</v>
       </c>
-      <c r="Y18" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z18" s="4">
-        <v>0.3</v>
+      <c r="Y18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.35">
@@ -2714,7 +2714,7 @@
         <v>86</v>
       </c>
       <c r="N19" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O19" s="4">
         <v>10</v>
@@ -2743,11 +2743,11 @@
       <c r="X19" s="3">
         <v>1</v>
       </c>
-      <c r="Y19" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z19" s="4">
-        <v>0.3</v>
+      <c r="Y19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.35">
@@ -2791,7 +2791,7 @@
         <v>86</v>
       </c>
       <c r="N20" s="4">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="O20" s="4">
         <v>10</v>
@@ -2820,11 +2820,11 @@
       <c r="X20" s="3">
         <v>1</v>
       </c>
-      <c r="Y20" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="Z20" s="4">
-        <v>0.3</v>
+      <c r="Y20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.35">
@@ -4991,6 +4991,9 @@
       </c>
       <c r="D50" s="7" t="s">
         <v>155</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0.5</v>
       </c>
       <c r="F50" s="4">
         <v>1250</v>

</xml_diff>

<commit_message>
Fix font size in tech selection plots
</commit_message>
<xml_diff>
--- a/es_gui/apps/data_manager/_static/techs_database.xlsx
+++ b/es_gui/apps/data_manager/_static/techs_database.xlsx
@@ -1113,16 +1113,15 @@
   <dimension ref="A1:CK51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T29" sqref="T29"/>
+      <selection pane="bottomRight" activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.81640625" style="3" customWidth="1"/>
+    <col min="1" max="2" width="37.81640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.54296875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" style="7" customWidth="1"/>
     <col min="5" max="5" width="10.54296875" style="4" customWidth="1"/>

</xml_diff>